<commit_message>
Resizee and Google Colaboratory
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Размеры изображения</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>512x512</t>
+  </si>
+  <si>
+    <t>55.56%</t>
+  </si>
+  <si>
+    <t>После ресайза</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,15 +820,33 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>450</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2">
+        <v>12</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>

</xml_diff>